<commit_message>
extract feedback to partials
</commit_message>
<xml_diff>
--- a/public/files/bulk_curation_template.xlsx
+++ b/public/files/bulk_curation_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jward3/projects/clingen/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{429CA52B-B824-6946-8299-4062A16D6A77}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29B9C451-12B4-F44E-808A-C71EB972E067}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
-  <si>
-    <t>rationale_notes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Assertion</t>
   </si>
@@ -97,24 +94,6 @@
     <t>Rationales</t>
   </si>
   <si>
-    <t>precuration_date</t>
-  </si>
-  <si>
-    <t>disease_entity_assigned_date</t>
-  </si>
-  <si>
-    <t>curation_provisional_date</t>
-  </si>
-  <si>
-    <t>curation_in_progress_date</t>
-  </si>
-  <si>
-    <t>curation_approved_date</t>
-  </si>
-  <si>
-    <t>disease_entity if there is no mondo id</t>
-  </si>
-  <si>
     <t>curation types</t>
   </si>
   <si>
@@ -151,9 +130,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Expert Panel Id</t>
-  </si>
-  <si>
     <t>Curator Email</t>
   </si>
   <si>
@@ -166,27 +142,6 @@
     <t>Curation Type</t>
   </si>
   <si>
-    <t>date_uploaded</t>
-  </si>
-  <si>
-    <t>BRCA1</t>
-  </si>
-  <si>
-    <t>sirs@unc.edu</t>
-  </si>
-  <si>
-    <t>notes on the rationale</t>
-  </si>
-  <si>
-    <t>BRCA2</t>
-  </si>
-  <si>
-    <t>test test test</t>
-  </si>
-  <si>
-    <t>MYL2</t>
-  </si>
-  <si>
     <t>OMIM ID 1</t>
   </si>
   <si>
@@ -217,16 +172,70 @@
     <t>OMIM ID 10</t>
   </si>
   <si>
-    <t>rationale 1</t>
-  </si>
-  <si>
-    <t>rationale 2</t>
-  </si>
-  <si>
-    <t>rationale 3</t>
-  </si>
-  <si>
-    <t>rationale 4</t>
+    <t>Disease entity if there is no mondo id</t>
+  </si>
+  <si>
+    <t>Rationale 1</t>
+  </si>
+  <si>
+    <t>Rationale 2</t>
+  </si>
+  <si>
+    <t>Rationale 3</t>
+  </si>
+  <si>
+    <t>Rationale 4</t>
+  </si>
+  <si>
+    <t>Rationale Notes</t>
+  </si>
+  <si>
+    <t>Date Uploaded</t>
+  </si>
+  <si>
+    <t>Precuration Date</t>
+  </si>
+  <si>
+    <t>Disease Entity Assigned Date</t>
+  </si>
+  <si>
+    <t>Curation In Progress Date</t>
+  </si>
+  <si>
+    <t>Curation Provisional Date</t>
+  </si>
+  <si>
+    <t>Curation Approved Date</t>
+  </si>
+  <si>
+    <t>PMID 1</t>
+  </si>
+  <si>
+    <t>PMID 2</t>
+  </si>
+  <si>
+    <t>PMID 3</t>
+  </si>
+  <si>
+    <t>PMID 4</t>
+  </si>
+  <si>
+    <t>PMID 5</t>
+  </si>
+  <si>
+    <t>PMID 6</t>
+  </si>
+  <si>
+    <t>PMID 7</t>
+  </si>
+  <si>
+    <t>PMID 8</t>
+  </si>
+  <si>
+    <t>PMID 9</t>
+  </si>
+  <si>
+    <t>PMID 10</t>
   </si>
 </sst>
 </file>
@@ -234,9 +243,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +273,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -318,9 +335,10 @@
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -682,758 +700,684 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3D26-773C-0343-9D4F-0C8AA45D4AC9}">
-  <dimension ref="A1:AA254"/>
+  <dimension ref="A1:AJ254"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="12" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" customWidth="1"/>
-    <col min="16" max="16" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="11" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="7.1640625" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="U1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="AF1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="AG1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="AH1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AI1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="10">
-        <v>93849384</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>2</v>
-      </c>
-      <c r="U2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="9">
-        <v>42370</v>
-      </c>
-      <c r="W2" s="9">
-        <v>42401</v>
-      </c>
-      <c r="X2" s="9">
-        <v>42401</v>
-      </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="10">
-        <v>98239823</v>
-      </c>
-      <c r="F3" s="11">
-        <v>29849283</v>
-      </c>
-      <c r="G3" s="11">
-        <v>29813918</v>
-      </c>
-      <c r="H3" s="11">
-        <v>198191281</v>
-      </c>
-      <c r="P3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="9">
-        <v>42860</v>
-      </c>
-      <c r="W3" s="9">
-        <v>42863</v>
-      </c>
-      <c r="X3" s="9">
-        <v>42864</v>
-      </c>
-      <c r="Y3" s="9">
-        <v>42865</v>
-      </c>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="10">
-        <v>18329238</v>
-      </c>
-      <c r="P4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" t="s">
-        <v>49</v>
-      </c>
-      <c r="V4" s="9">
-        <v>42860</v>
-      </c>
-      <c r="W4" s="9">
-        <v>42863</v>
-      </c>
-      <c r="X4" s="9">
-        <v>42864</v>
-      </c>
-      <c r="Y4" s="9">
-        <v>42865</v>
-      </c>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B2" s="8"/>
+      <c r="D2" s="10"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="D4" s="10"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-      <c r="AA13" s="9"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+    </row>
+    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+    </row>
+    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+    </row>
+    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+    </row>
+    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+    </row>
+    <row r="21" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+    </row>
+    <row r="22" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+    </row>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+    </row>
+    <row r="24" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+    </row>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+    </row>
+    <row r="26" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+    </row>
+    <row r="27" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+    </row>
+    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+    </row>
+    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="9"/>
+      <c r="AJ30" s="9"/>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-    </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
+      <c r="AJ32" s="9"/>
+    </row>
+    <row r="33" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-      <c r="AA33" s="9"/>
-    </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE33" s="9"/>
+      <c r="AF33" s="9"/>
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="9"/>
+      <c r="AI33" s="9"/>
+      <c r="AJ33" s="9"/>
+    </row>
+    <row r="34" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="Y34" s="9"/>
-      <c r="Z34" s="9"/>
-      <c r="AA34" s="9"/>
-    </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE34" s="9"/>
+      <c r="AF34" s="9"/>
+      <c r="AG34" s="9"/>
+      <c r="AH34" s="9"/>
+      <c r="AI34" s="9"/>
+      <c r="AJ34" s="9"/>
+    </row>
+    <row r="35" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="9"/>
-    </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="9"/>
+      <c r="AG35" s="9"/>
+      <c r="AH35" s="9"/>
+      <c r="AI35" s="9"/>
+      <c r="AJ35" s="9"/>
+    </row>
+    <row r="36" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-    </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE36" s="9"/>
+      <c r="AF36" s="9"/>
+      <c r="AG36" s="9"/>
+      <c r="AH36" s="9"/>
+      <c r="AI36" s="9"/>
+      <c r="AJ36" s="9"/>
+    </row>
+    <row r="37" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AA37" s="9"/>
-    </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE37" s="9"/>
+      <c r="AF37" s="9"/>
+      <c r="AG37" s="9"/>
+      <c r="AH37" s="9"/>
+      <c r="AI37" s="9"/>
+      <c r="AJ37" s="9"/>
+    </row>
+    <row r="38" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B38" s="5"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
-      <c r="X38" s="9"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="9"/>
-      <c r="AA38" s="9"/>
-    </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE38" s="9"/>
+      <c r="AF38" s="9"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="9"/>
+      <c r="AI38" s="9"/>
+      <c r="AJ38" s="9"/>
+    </row>
+    <row r="39" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
-      <c r="AA39" s="9"/>
-    </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="9"/>
+      <c r="AI39" s="9"/>
+      <c r="AJ39" s="9"/>
+    </row>
+    <row r="40" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B40" s="5"/>
-      <c r="V40" s="9"/>
-      <c r="W40" s="9"/>
-      <c r="X40" s="9"/>
-      <c r="Y40" s="9"/>
-      <c r="Z40" s="9"/>
-      <c r="AA40" s="9"/>
-    </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+      <c r="AG40" s="9"/>
+      <c r="AH40" s="9"/>
+      <c r="AI40" s="9"/>
+      <c r="AJ40" s="9"/>
+    </row>
+    <row r="41" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B41" s="5"/>
-      <c r="V41" s="9"/>
-      <c r="W41" s="9"/>
-      <c r="X41" s="9"/>
-      <c r="Y41" s="9"/>
-      <c r="Z41" s="9"/>
-      <c r="AA41" s="9"/>
-    </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE41" s="9"/>
+      <c r="AF41" s="9"/>
+      <c r="AG41" s="9"/>
+      <c r="AH41" s="9"/>
+      <c r="AI41" s="9"/>
+      <c r="AJ41" s="9"/>
+    </row>
+    <row r="42" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B42" s="5"/>
-      <c r="V42" s="9"/>
-      <c r="W42" s="9"/>
-      <c r="X42" s="9"/>
-      <c r="Y42" s="9"/>
-      <c r="Z42" s="9"/>
-      <c r="AA42" s="9"/>
-    </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE42" s="9"/>
+      <c r="AF42" s="9"/>
+      <c r="AG42" s="9"/>
+      <c r="AH42" s="9"/>
+      <c r="AI42" s="9"/>
+      <c r="AJ42" s="9"/>
+    </row>
+    <row r="43" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B43" s="5"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="9"/>
-      <c r="AA43" s="9"/>
-    </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="9"/>
+      <c r="AG43" s="9"/>
+      <c r="AH43" s="9"/>
+      <c r="AI43" s="9"/>
+      <c r="AJ43" s="9"/>
+    </row>
+    <row r="44" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B44" s="5"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
-      <c r="AA44" s="9"/>
-    </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE44" s="9"/>
+      <c r="AF44" s="9"/>
+      <c r="AG44" s="9"/>
+      <c r="AH44" s="9"/>
+      <c r="AI44" s="9"/>
+      <c r="AJ44" s="9"/>
+    </row>
+    <row r="45" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B45" s="5"/>
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="9"/>
-      <c r="Y45" s="9"/>
-      <c r="Z45" s="9"/>
-      <c r="AA45" s="9"/>
-    </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE45" s="9"/>
+      <c r="AF45" s="9"/>
+      <c r="AG45" s="9"/>
+      <c r="AH45" s="9"/>
+      <c r="AI45" s="9"/>
+      <c r="AJ45" s="9"/>
+    </row>
+    <row r="46" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B46" s="5"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="9"/>
-      <c r="Z46" s="9"/>
-      <c r="AA46" s="9"/>
-    </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="9"/>
+      <c r="AG46" s="9"/>
+      <c r="AH46" s="9"/>
+      <c r="AI46" s="9"/>
+      <c r="AJ46" s="9"/>
+    </row>
+    <row r="47" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B47" s="5"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
-      <c r="X47" s="9"/>
-      <c r="Y47" s="9"/>
-      <c r="Z47" s="9"/>
-      <c r="AA47" s="9"/>
-    </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="9"/>
+      <c r="AG47" s="9"/>
+      <c r="AH47" s="9"/>
+      <c r="AI47" s="9"/>
+      <c r="AJ47" s="9"/>
+    </row>
+    <row r="48" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
-      <c r="V48" s="9"/>
-      <c r="W48" s="9"/>
-      <c r="X48" s="9"/>
-      <c r="Y48" s="9"/>
-      <c r="Z48" s="9"/>
-      <c r="AA48" s="9"/>
-    </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
+      <c r="AG48" s="9"/>
+      <c r="AH48" s="9"/>
+      <c r="AI48" s="9"/>
+      <c r="AJ48" s="9"/>
+    </row>
+    <row r="49" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="9"/>
-      <c r="Y49" s="9"/>
-      <c r="Z49" s="9"/>
-      <c r="AA49" s="9"/>
-    </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE49" s="9"/>
+      <c r="AF49" s="9"/>
+      <c r="AG49" s="9"/>
+      <c r="AH49" s="9"/>
+      <c r="AI49" s="9"/>
+      <c r="AJ49" s="9"/>
+    </row>
+    <row r="50" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B50" s="5"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="9"/>
-      <c r="Z50" s="9"/>
-      <c r="AA50" s="9"/>
-    </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="9"/>
+      <c r="AH50" s="9"/>
+      <c r="AI50" s="9"/>
+      <c r="AJ50" s="9"/>
+    </row>
+    <row r="51" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="9"/>
-      <c r="Z51" s="9"/>
-      <c r="AA51" s="9"/>
-    </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="9"/>
+      <c r="AG51" s="9"/>
+      <c r="AH51" s="9"/>
+      <c r="AI51" s="9"/>
+      <c r="AJ51" s="9"/>
+    </row>
+    <row r="52" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B52" s="5"/>
-      <c r="V52" s="9"/>
-      <c r="W52" s="9"/>
-      <c r="X52" s="9"/>
-      <c r="Y52" s="9"/>
-      <c r="Z52" s="9"/>
-      <c r="AA52" s="9"/>
-    </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE52" s="9"/>
+      <c r="AF52" s="9"/>
+      <c r="AG52" s="9"/>
+      <c r="AH52" s="9"/>
+      <c r="AI52" s="9"/>
+      <c r="AJ52" s="9"/>
+    </row>
+    <row r="53" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
-      <c r="X53" s="9"/>
-      <c r="Y53" s="9"/>
-      <c r="Z53" s="9"/>
-      <c r="AA53" s="9"/>
-    </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE53" s="9"/>
+      <c r="AF53" s="9"/>
+      <c r="AG53" s="9"/>
+      <c r="AH53" s="9"/>
+      <c r="AI53" s="9"/>
+      <c r="AJ53" s="9"/>
+    </row>
+    <row r="54" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B54" s="5"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="9"/>
-      <c r="Z54" s="9"/>
-      <c r="AA54" s="9"/>
-    </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
+      <c r="AI54" s="9"/>
+      <c r="AJ54" s="9"/>
+    </row>
+    <row r="55" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B55" s="5"/>
-      <c r="V55" s="9"/>
-      <c r="W55" s="9"/>
-      <c r="X55" s="9"/>
-      <c r="Y55" s="9"/>
-      <c r="Z55" s="9"/>
-      <c r="AA55" s="9"/>
-    </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
+      <c r="AI55" s="9"/>
+      <c r="AJ55" s="9"/>
+    </row>
+    <row r="56" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B56" s="5"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="9"/>
-      <c r="Z56" s="9"/>
-      <c r="AA56" s="9"/>
-    </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="9"/>
+      <c r="AG56" s="9"/>
+      <c r="AH56" s="9"/>
+      <c r="AI56" s="9"/>
+      <c r="AJ56" s="9"/>
+    </row>
+    <row r="57" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B57" s="5"/>
-      <c r="V57" s="9"/>
-      <c r="W57" s="9"/>
-      <c r="X57" s="9"/>
-      <c r="Y57" s="9"/>
-      <c r="Z57" s="9"/>
-      <c r="AA57" s="9"/>
-    </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="9"/>
+      <c r="AG57" s="9"/>
+      <c r="AH57" s="9"/>
+      <c r="AI57" s="9"/>
+      <c r="AJ57" s="9"/>
+    </row>
+    <row r="58" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B58" s="5"/>
-      <c r="V58" s="9"/>
-      <c r="W58" s="9"/>
-      <c r="X58" s="9"/>
-      <c r="Y58" s="9"/>
-      <c r="Z58" s="9"/>
-      <c r="AA58" s="9"/>
-    </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE58" s="9"/>
+      <c r="AF58" s="9"/>
+      <c r="AG58" s="9"/>
+      <c r="AH58" s="9"/>
+      <c r="AI58" s="9"/>
+      <c r="AJ58" s="9"/>
+    </row>
+    <row r="59" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
-      <c r="X59" s="9"/>
-      <c r="Y59" s="9"/>
-      <c r="Z59" s="9"/>
-      <c r="AA59" s="9"/>
-    </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AE59" s="9"/>
+      <c r="AF59" s="9"/>
+      <c r="AG59" s="9"/>
+      <c r="AH59" s="9"/>
+      <c r="AI59" s="9"/>
+      <c r="AJ59" s="9"/>
+    </row>
+    <row r="60" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B60" s="5"/>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B62" s="5"/>
     </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B64" s="5"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
@@ -2007,11 +1951,6 @@
       <c r="B254" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A80EC79B-2F5D-8F44-B6B0-940454424882}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{B36354CF-ECBE-8846-A16E-88DC87860498}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{DF605ACA-064E-9F45-AC4B-73E8A56122D1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
@@ -2021,13 +1960,13 @@
           <x14:formula1>
             <xm:f>lookups!$L$3:$L$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0726DCE-314E-1F40-BD9F-58E32A57A97C}">
           <x14:formula1>
             <xm:f>lookups!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>Q5:Q144 Q2:T4 R5:T178</xm:sqref>
+          <xm:sqref>P5:P144 P2:S4 Q5:S178</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2060,50 +1999,50 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2111,34 +2050,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -2146,33 +2085,33 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2180,33 +2119,33 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5">
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2214,33 +2153,33 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2248,13 +2187,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -2263,13 +2202,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -2278,14 +2217,14 @@
         <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2296,7 +2235,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2307,7 +2246,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2318,7 +2257,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2329,7 +2268,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>

</xml_diff>

<commit_message>
Fix typo in curation_type name
</commit_message>
<xml_diff>
--- a/public/files/bulk_curation_template.xlsx
+++ b/public/files/bulk_curation_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jward3/projects/clingen/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29B9C451-12B4-F44E-808A-C71EB972E067}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D802F53-F0AE-8649-8918-C9647D061E11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
   </bookViews>
   <sheets>
     <sheet name="Curations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Assertion</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>PMID 10</t>
+  </si>
+  <si>
+    <t>isolated-phenotype</t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3D26-773C-0343-9D4F-0C8AA45D4AC9}">
   <dimension ref="A1:AJ254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+    <sheetView topLeftCell="T1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -1978,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2336B327-67B0-B54C-8AB1-1809F42E0D2F}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1994,6 +1997,7 @@
     <col min="9" max="9" width="36.5" customWidth="1"/>
     <col min="10" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="65.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2132,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
fix bulk upload template
</commit_message>
<xml_diff>
--- a/public/files/bulk_curation_template.xlsx
+++ b/public/files/bulk_curation_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jward3/projects/clingen/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D802F53-F0AE-8649-8918-C9647D061E11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A92A14BA-CBA1-FB44-9A08-267D20EC27F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Assertion</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>single-new</t>
-  </si>
-  <si>
-    <t>isoloted-phenotype</t>
   </si>
   <si>
     <t>lumped</t>
@@ -383,18 +380,6 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A102D704-4E04-7C41-BE73-2426AD31AEC4}" name="Table3" displayName="Table3" ref="K2:M7" totalsRowShown="0">
-  <autoFilter ref="K2:M7" xr:uid="{C176C88B-5B74-4F4B-B381-A3DB332913DC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6A67F328-C5A3-B046-B904-C91A32C9DD2E}" name="id"/>
-    <tableColumn id="2" xr3:uid="{A8437228-08D8-C14E-ADD1-7DD24AEC3545}" name="name"/>
-    <tableColumn id="3" xr3:uid="{C5C59AD8-2D30-C74E-A965-F8375581C2C6}" name="Description"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7D7B7710-9121-2C4E-B591-4E55B84CC9CA}" name="Table36" displayName="Table36" ref="G2:I7" totalsRowShown="0">
   <autoFilter ref="G2:I7" xr:uid="{5E786F4B-029A-664E-A78E-578529E1EFB3}"/>
   <tableColumns count="3">
@@ -705,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3D26-773C-0343-9D4F-0C8AA45D4AC9}">
   <dimension ref="A1:AJ254"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,112 +720,112 @@
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -1961,7 +1946,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{29A5C92E-2A51-8845-96FE-684BC3DDCAE2}">
           <x14:formula1>
-            <xm:f>lookups!$L$3:$L$6</xm:f>
+            <xm:f>lookups!$H$3:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1979,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2336B327-67B0-B54C-8AB1-1809F42E0D2F}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1994,14 +1979,14 @@
     <col min="6" max="6" width="6.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.5" customWidth="1"/>
+    <col min="9" max="9" width="65.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="65.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
@@ -2012,11 +1997,9 @@
       <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2037,19 +2020,10 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2071,20 +2045,11 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2105,20 +2070,11 @@
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2136,23 +2092,14 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2170,23 +2117,14 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2201,7 +2139,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2216,7 +2154,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -2233,7 +2171,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10" s="2"/>
       <c r="D10">
         <v>8</v>
@@ -2244,7 +2182,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" s="2"/>
       <c r="D11">
         <v>9</v>
@@ -2255,7 +2193,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C12" s="2"/>
       <c r="D12">
         <v>10</v>
@@ -2266,7 +2204,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13">
         <v>11</v>
@@ -2277,13 +2215,13 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
       <c r="E15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2307,11 +2245,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>